<commit_message>
Leetcode problem Is subsequence
</commit_message>
<xml_diff>
--- a/LeetCode-Neetcode.xlsx
+++ b/LeetCode-Neetcode.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbhagwat/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbhagwat/Downloads/Leetcode-Handpicked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{039223BD-331C-794B-9B43-CE840B62DAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9DC77E-E08D-0647-A36F-C1E41749846C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{BD01C3DC-DC56-CE43-9723-FA137E1E129F}"/>
+    <workbookView xWindow="7900" yWindow="3260" windowWidth="28040" windowHeight="17440" xr2:uid="{BD01C3DC-DC56-CE43-9723-FA137E1E129F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Leetcode Problems</t>
   </si>
@@ -48,6 +48,24 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/is-subsequence/solutions/</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/length-of-last-word/</t>
+  </si>
+  <si>
+    <t>Hashmap &amp; Hashset</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contains-duplicate/</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/concatenation-of-array/description/</t>
   </si>
 </sst>
 </file>
@@ -447,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7297CB5-68C8-6E42-888B-4EB2556D0AF9}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,10 +496,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{2B8E9F3C-D672-404F-8E29-B3B61436DB9A}"/>
     <hyperlink ref="A6" r:id="rId2" xr:uid="{F5FD0255-5A65-6740-A239-5A889FBC806E}"/>
+    <hyperlink ref="A10" r:id="rId3" xr:uid="{00A9F9BF-33C1-0E41-9C76-CB7AF24BC48D}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{FCDB55F0-13E0-5E42-9598-01FFB8BD2220}"/>
+    <hyperlink ref="A19" r:id="rId5" xr:uid="{97D07EA3-D1DA-8248-9CFB-806E6CCD565B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Leetcode problem two sum and others
</commit_message>
<xml_diff>
--- a/LeetCode-Neetcode.xlsx
+++ b/LeetCode-Neetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahulbhagwat/Downloads/Leetcode-Handpicked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9DC77E-E08D-0647-A36F-C1E41749846C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF66D2BE-A9CC-5742-9A49-E744DA9D1A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="3260" windowWidth="28040" windowHeight="17440" xr2:uid="{BD01C3DC-DC56-CE43-9723-FA137E1E129F}"/>
+    <workbookView xWindow="2200" yWindow="1040" windowWidth="28040" windowHeight="17440" xr2:uid="{BD01C3DC-DC56-CE43-9723-FA137E1E129F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Leetcode Problems</t>
   </si>
@@ -50,9 +50,6 @@
     <t>https://leetcode.com/problems/is-subsequence/solutions/</t>
   </si>
   <si>
-    <t>Strings</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/length-of-last-word/</t>
   </si>
   <si>
@@ -66,6 +63,33 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/concatenation-of-array/description/</t>
+  </si>
+  <si>
+    <t>String Manipulation</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/two-sum/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-anagram/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-senior-citizens/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/max-consecutive-ones/</t>
+  </si>
+  <si>
+    <t>Sliding Window</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/score-of-a-string/</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>keep count of 1s and increase the window when we find subs ones …..reset window when no subs ones</t>
   </si>
 </sst>
 </file>
@@ -465,65 +489,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7297CB5-68C8-6E42-888B-4EB2556D0AF9}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="88.33203125" customWidth="1"/>
+    <col min="2" max="2" width="110.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>9</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -533,6 +594,11 @@
     <hyperlink ref="A10" r:id="rId3" xr:uid="{00A9F9BF-33C1-0E41-9C76-CB7AF24BC48D}"/>
     <hyperlink ref="A14" r:id="rId4" xr:uid="{FCDB55F0-13E0-5E42-9598-01FFB8BD2220}"/>
     <hyperlink ref="A19" r:id="rId5" xr:uid="{97D07EA3-D1DA-8248-9CFB-806E6CCD565B}"/>
+    <hyperlink ref="A15" r:id="rId6" xr:uid="{E7D24FC1-A02B-D14D-B99A-26A2CEEB2039}"/>
+    <hyperlink ref="A16" r:id="rId7" xr:uid="{E66837C5-113B-9B49-A4F7-E745540AF1C4}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{8A796CC3-5B50-A348-B439-FB6301CB5594}"/>
+    <hyperlink ref="A23" r:id="rId9" xr:uid="{F3C2E31B-4ECA-C84F-B1EB-486BA7D92942}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{101A27B8-5BA5-294B-AC30-5AA92009B1F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>